<commit_message>
[제품]  상세이미지 check - On going
</commit_message>
<xml_diff>
--- a/제품등록 검토사항.xlsx
+++ b/제품등록 검토사항.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="등록방법" sheetId="2" r:id="rId1"/>
@@ -680,7 +680,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -858,11 +858,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -916,46 +1086,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3229,8 +3483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3464,7 +3718,7 @@
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="30" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -3481,7 +3735,7 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="21"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="18" t="s">
         <v>81</v>
       </c>
@@ -3496,7 +3750,7 @@
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="21"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
@@ -3511,7 +3765,7 @@
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="21"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
@@ -3526,7 +3780,7 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="21"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="18" t="s">
         <v>84</v>
       </c>
@@ -3541,7 +3795,7 @@
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="21"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="18" t="s">
         <v>85</v>
       </c>
@@ -3556,7 +3810,7 @@
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="30" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -3573,7 +3827,7 @@
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="21"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="18" t="s">
         <v>88</v>
       </c>
@@ -3605,16 +3859,16 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>50002032</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="31">
         <v>50</v>
       </c>
       <c r="F15" s="20">
@@ -3622,72 +3876,72 @@
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>50002265</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="20">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="21"/>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>50002384</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="21"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>50002267</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="21"/>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>50002380</v>
       </c>
-      <c r="E19" s="23"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="21"/>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>50002605</v>
       </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="30" t="s">
         <v>98</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -3696,7 +3950,7 @@
       <c r="D21" s="18">
         <v>50002266</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="31">
         <v>11</v>
       </c>
       <c r="F21" s="20">
@@ -3704,166 +3958,166 @@
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="21"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="18" t="s">
         <v>100</v>
       </c>
       <c r="D22" s="18">
         <v>50004797</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24">
+      <c r="E22" s="31"/>
+      <c r="F22" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="23">
         <v>50002006</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="31">
         <v>21</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="21"/>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="23">
         <v>50002384</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24">
+      <c r="E24" s="31"/>
+      <c r="F24" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="21"/>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="21">
         <v>50002595</v>
       </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24">
+      <c r="E25" s="31"/>
+      <c r="F25" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="21"/>
-      <c r="C26" s="22" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>50002596</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24">
+      <c r="E26" s="31"/>
+      <c r="F26" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22" t="s">
+      <c r="B27" s="30"/>
+      <c r="C27" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="21">
         <v>50002267</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24">
+      <c r="E27" s="31"/>
+      <c r="F27" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="21">
         <v>50002380</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24">
+      <c r="E28" s="31"/>
+      <c r="F28" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="21"/>
-      <c r="C29" s="22" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="21">
         <v>50002606</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24">
+      <c r="E29" s="31"/>
+      <c r="F29" s="22">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22" t="s">
+      <c r="B30" s="30"/>
+      <c r="C30" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="21">
         <v>50002607</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24">
+      <c r="E30" s="31"/>
+      <c r="F30" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="21">
         <v>50002267</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="31">
         <v>40</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="22">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="21"/>
-      <c r="C32" s="22" t="s">
+      <c r="B32" s="30"/>
+      <c r="C32" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="21">
         <v>50002606</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="24">
+      <c r="E32" s="31"/>
+      <c r="F32" s="22">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="21"/>
-      <c r="C33" s="22" t="s">
+      <c r="B33" s="30"/>
+      <c r="C33" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="21">
         <v>50002607</v>
       </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24">
+      <c r="E33" s="31"/>
+      <c r="F33" s="22">
         <v>4</v>
       </c>
     </row>
@@ -3871,10 +4125,10 @@
       <c r="B34" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="21">
         <v>50002606</v>
       </c>
       <c r="E34" s="19">
@@ -3902,115 +4156,121 @@
       </c>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="21">
         <v>50002384</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="31">
         <v>67</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="22">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="21"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D37" s="18">
         <v>50002268</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="24">
+      <c r="E37" s="31"/>
+      <c r="F37" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="21"/>
-      <c r="C38" s="25" t="s">
+      <c r="B38" s="30"/>
+      <c r="C38" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="23">
         <v>50002594</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="24">
+      <c r="E38" s="31"/>
+      <c r="F38" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="21"/>
-      <c r="C39" s="25" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="25">
+      <c r="D39" s="23">
         <v>50002596</v>
       </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24">
+      <c r="E39" s="31"/>
+      <c r="F39" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="2:6">
-      <c r="B40" s="21"/>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="21">
         <v>50002267</v>
       </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="24">
+      <c r="E40" s="31"/>
+      <c r="F40" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:6">
-      <c r="B41" s="21"/>
-      <c r="C41" s="25" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="23">
         <v>50002381</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="24">
+      <c r="E41" s="31"/>
+      <c r="F41" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="2:6">
-      <c r="B42" s="21"/>
-      <c r="C42" s="25" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="23">
         <v>50002380</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="24">
+      <c r="E42" s="31"/>
+      <c r="F42" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29">
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="24">
         <f>SUM(E4:E42)</f>
         <v>537</v>
       </c>
-      <c r="F43" s="30">
+      <c r="F43" s="25">
         <f>SUM(F4:F42)</f>
         <v>535</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="E23:E30"/>
@@ -4018,12 +4278,6 @@
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="B36:B42"/>
     <mergeCell ref="E36:E42"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:E22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4034,8 +4288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4062,7 +4316,7 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="26" t="s">
         <v>98</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -4071,12 +4325,12 @@
       <c r="D4" s="18">
         <v>50004797</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -4118,7 +4372,7 @@
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -4132,7 +4386,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="18" t="s">
@@ -4146,7 +4400,7 @@
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -4169,26 +4423,26 @@
       <c r="D11" s="33">
         <v>50002008</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="22">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="23">
         <v>50002006</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -4201,417 +4455,417 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="31" t="s">
+    <row r="14" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B14" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="35">
         <v>50002001</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="36">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="48">
         <v>50001998</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="49">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="17" t="s">
+    <row r="16" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B16" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="51">
         <v>50001998</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="52">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="41">
         <v>50002455</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>50002032</v>
       </c>
       <c r="E18" s="20">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="31" t="s">
+    <row r="19" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B19" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="37">
         <v>50002265</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="36">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="53">
         <v>50002384</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="49">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="23">
         <v>50002384</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="31" t="s">
+    <row r="22" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B22" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="55">
         <v>50002384</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="56">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="41">
         <v>50002268</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="43">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="31" t="s">
+    <row r="24" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B24" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="38">
         <v>50002594</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="39">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="53">
         <v>50002595</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="57">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>50002596</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B27" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="58">
         <v>50002596</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="56">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="53">
         <v>50002267</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="49">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="21">
         <v>50002267</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="21">
         <v>50002267</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="22">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="31" t="s">
+    <row r="31" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B31" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="55">
         <v>50002267</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="56">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="31" t="s">
+    <row r="32" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B32" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="45">
         <v>50002381</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="46">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="53">
         <v>50002380</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="49">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="21">
         <v>50002380</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="22">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="31" t="s">
+    <row r="35" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B35" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="58">
         <v>50002380</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="56">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="41">
         <v>50002266</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="42">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="31" t="s">
+    <row r="37" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B37" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="37">
         <v>50002605</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="36">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="53">
         <v>50002606</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="57">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="21">
         <v>50002606</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="17" t="s">
+    <row r="40" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B40" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="55">
         <v>50002606</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="52">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="53">
         <v>50002607</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="57">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="31" t="s">
+    <row r="42" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B42" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="55">
         <v>50002607</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="56">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="30">
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62">
         <f>SUM(E4:E42)</f>
         <v>535</v>
       </c>

</xml_diff>